<commit_message>
UPDATE noede2vec and line
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qianzhiqiang/PycharmProjects/NetBenchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA83AB6-895F-384F-B885-83B5C4776146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEE38A8-D9C9-824F-A5A8-7C9CD9770EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="520" windowWidth="28240" windowHeight="16400" xr2:uid="{A9C37B03-D3ED-DD4C-96A1-B014332CD34F}"/>
   </bookViews>
@@ -164,7 +164,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -196,19 +196,31 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u val="double"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="double"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -225,11 +237,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -249,6 +258,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,60 +588,64 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="12" max="13" width="10.83203125" style="9"/>
+    <col min="16" max="17" width="10.83203125" style="9"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="5" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="5" t="s">
+      <c r="K1" s="5"/>
+      <c r="L1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="5"/>
-      <c r="N1" s="4" t="s">
+      <c r="M1" s="7"/>
+      <c r="N1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4" t="s">
+      <c r="O1" s="3"/>
+      <c r="P1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4" t="s">
+      <c r="Q1" s="10"/>
+      <c r="R1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4" t="s">
+      <c r="S1" s="3"/>
+      <c r="T1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="U1" s="3"/>
+      <c r="V1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4" t="s">
+      <c r="W1" s="3"/>
+      <c r="X1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="4"/>
+      <c r="Y1" s="3"/>
     </row>
     <row r="2" spans="1:25">
       <c r="B2" t="s">
@@ -653,10 +678,10 @@
       <c r="K2" t="s">
         <v>19</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="8" t="s">
         <v>19</v>
       </c>
       <c r="N2" t="s">
@@ -665,10 +690,10 @@
       <c r="O2" t="s">
         <v>19</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="8" t="s">
         <v>19</v>
       </c>
       <c r="R2" t="s">
@@ -730,10 +755,10 @@
       <c r="K3">
         <v>0.70020000000000004</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="8">
         <v>0.97450000000000003</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="8">
         <v>0.56789999999999996</v>
       </c>
       <c r="N3">
@@ -742,10 +767,10 @@
       <c r="O3">
         <v>0.84450000000000003</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="8">
         <v>0.67710000000000004</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="Q3" s="8">
         <v>4.8099999999999997E-2</v>
       </c>
       <c r="R3">
@@ -807,10 +832,10 @@
       <c r="K4">
         <v>0.67020000000000002</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="8">
         <v>0.85699999999999998</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="8">
         <v>4.36E-2</v>
       </c>
       <c r="N4">
@@ -819,10 +844,10 @@
       <c r="O4">
         <v>0.80889999999999995</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="8">
         <v>0.67689999999999995</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="Q4" s="8">
         <v>4.8300000000000003E-2</v>
       </c>
       <c r="R4">
@@ -884,10 +909,10 @@
       <c r="K5">
         <v>0.46679999999999999</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="8">
         <v>0.85780000000000001</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="8">
         <v>4.7800000000000002E-2</v>
       </c>
       <c r="N5">
@@ -896,10 +921,10 @@
       <c r="O5">
         <v>0.74839999999999995</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="8">
         <v>0.67589999999999995</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="Q5" s="8">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="R5">
@@ -961,12 +986,16 @@
       <c r="K6">
         <v>0.57620000000000005</v>
       </c>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
       <c r="N6">
         <v>0.83420000000000005</v>
       </c>
       <c r="O6">
         <v>0.82299999999999995</v>
       </c>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
       <c r="R6">
         <v>0.66439999999999999</v>
       </c>
@@ -1014,6 +1043,10 @@
       <c r="G7">
         <v>0.71930000000000005</v>
       </c>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
       <c r="R7">
         <v>0.68200000000000005</v>
       </c>
@@ -1073,10 +1106,10 @@
       <c r="K8">
         <v>0.71279999999999999</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="8">
         <v>0.94210000000000005</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="8">
         <v>0.2833</v>
       </c>
       <c r="N8">
@@ -1085,10 +1118,10 @@
       <c r="O8">
         <v>0.84689999999999999</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="8">
         <v>0.68969999999999998</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="8">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="R8">
@@ -1117,18 +1150,24 @@
       </c>
     </row>
     <row r="9" spans="1:25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="P10">
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="P10" s="8">
         <v>0.67579999999999996</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="8">
         <v>3.5400000000000001E-2</v>
       </c>
       <c r="R10">
@@ -1190,10 +1229,10 @@
       <c r="K11">
         <v>0.60060000000000002</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="8">
         <v>0.85799999999999998</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="8">
         <v>4.48E-2</v>
       </c>
       <c r="N11">
@@ -1202,14 +1241,88 @@
       <c r="O11">
         <v>0.82130000000000003</v>
       </c>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
     </row>
     <row r="12" spans="1:25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
+      <c r="B12">
+        <v>0.85370000000000001</v>
+      </c>
+      <c r="C12">
+        <v>0.84330000000000005</v>
+      </c>
+      <c r="D12">
+        <v>0.63449999999999995</v>
+      </c>
+      <c r="E12">
+        <v>0.63039999999999996</v>
+      </c>
+      <c r="F12">
+        <v>0.72170000000000001</v>
+      </c>
+      <c r="G12">
+        <v>0.71260000000000001</v>
+      </c>
+      <c r="H12">
+        <v>0.72870000000000001</v>
+      </c>
+      <c r="I12">
+        <v>0.66349999999999998</v>
+      </c>
+      <c r="J12">
+        <v>0.71530000000000005</v>
+      </c>
+      <c r="K12">
+        <v>0.67320000000000002</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0.85850000000000004</v>
+      </c>
+      <c r="M12" s="8">
+        <v>5.11E-2</v>
+      </c>
+      <c r="N12">
+        <v>0.83120000000000005</v>
+      </c>
+      <c r="O12">
+        <v>0.82050000000000001</v>
+      </c>
+      <c r="P12" s="8">
+        <v>0.67730000000000001</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>5.0500000000000003E-2</v>
+      </c>
+      <c r="R12">
+        <v>0.68589999999999995</v>
+      </c>
+      <c r="S12">
+        <v>0.68969999999999998</v>
+      </c>
+      <c r="T12">
+        <v>0.43070000000000003</v>
+      </c>
+      <c r="U12">
+        <v>0.25750000000000001</v>
+      </c>
+      <c r="V12">
+        <v>0.2409</v>
+      </c>
+      <c r="W12">
+        <v>0.17560000000000001</v>
+      </c>
+      <c r="X12">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="Y12">
+        <v>0.56299999999999994</v>
+      </c>
     </row>
     <row r="13" spans="1:25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D13">
@@ -1236,24 +1349,26 @@
       <c r="K13">
         <v>0.78449999999999998</v>
       </c>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1282,60 +1397,60 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView zoomScale="138" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4" t="s">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4" t="s">
+      <c r="O1" s="3"/>
+      <c r="P1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4" t="s">
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4" t="s">
+      <c r="S1" s="3"/>
+      <c r="T1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="U1" s="3"/>
+      <c r="V1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4" t="s">
+      <c r="W1" s="3"/>
+      <c r="X1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="4"/>
+      <c r="Y1" s="3"/>
     </row>
     <row r="2" spans="1:25">
       <c r="B2" t="s">
@@ -1460,10 +1575,10 @@
       <c r="P3">
         <v>0.98119999999999996</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="1">
         <v>0.97050000000000003</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="1">
         <v>0.99019999999999997</v>
       </c>
       <c r="S3">
@@ -1867,6 +1982,48 @@
     <row r="12" spans="1:25">
       <c r="A12" t="s">
         <v>25</v>
+      </c>
+      <c r="B12">
+        <v>0.99739999999999995</v>
+      </c>
+      <c r="C12">
+        <v>0.99629999999999996</v>
+      </c>
+      <c r="D12">
+        <v>0.91249999999999998</v>
+      </c>
+      <c r="E12">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="F12">
+        <v>0.94610000000000005</v>
+      </c>
+      <c r="G12">
+        <v>0.93589999999999995</v>
+      </c>
+      <c r="H12">
+        <v>0.99760000000000004</v>
+      </c>
+      <c r="I12">
+        <v>0.99709999999999999</v>
+      </c>
+      <c r="J12">
+        <v>0.99819999999999998</v>
+      </c>
+      <c r="K12">
+        <v>0.99770000000000003</v>
+      </c>
+      <c r="L12">
+        <v>0.98860000000000003</v>
+      </c>
+      <c r="M12">
+        <v>0.96609999999999996</v>
+      </c>
+      <c r="N12">
+        <v>0.99670000000000003</v>
+      </c>
+      <c r="O12">
+        <v>0.99519999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1930,61 +2087,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49071FE1-A904-7348-BAAE-72F9A46C7610}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView zoomScale="139" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4" t="s">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4" t="s">
+      <c r="O1" s="3"/>
+      <c r="P1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4" t="s">
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4" t="s">
+      <c r="S1" s="3"/>
+      <c r="T1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="U1" s="3"/>
+      <c r="V1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4" t="s">
+      <c r="W1" s="3"/>
+      <c r="X1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="4"/>
+      <c r="Y1" s="3"/>
     </row>
     <row r="2" spans="1:25">
       <c r="B2" t="s">
@@ -2097,19 +2254,19 @@
       <c r="L3">
         <v>0.97719999999999996</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <v>0.61450000000000005</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="1">
         <v>0.8619</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="1">
         <v>0.85899999999999999</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="1">
         <v>0.67669999999999997</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="1">
         <v>4.5900000000000003E-2</v>
       </c>
       <c r="R3">
@@ -2522,6 +2679,78 @@
     <row r="12" spans="1:25">
       <c r="A12" t="s">
         <v>25</v>
+      </c>
+      <c r="B12">
+        <v>0.85</v>
+      </c>
+      <c r="C12">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="D12">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="E12">
+        <v>0.64029999999999998</v>
+      </c>
+      <c r="F12">
+        <v>0.71719999999999995</v>
+      </c>
+      <c r="G12">
+        <v>0.70809999999999995</v>
+      </c>
+      <c r="H12">
+        <v>0.72670000000000001</v>
+      </c>
+      <c r="I12">
+        <v>0.66120000000000001</v>
+      </c>
+      <c r="J12">
+        <v>0.70209999999999995</v>
+      </c>
+      <c r="K12">
+        <v>0.65820000000000001</v>
+      </c>
+      <c r="L12">
+        <v>0.85870000000000002</v>
+      </c>
+      <c r="M12">
+        <v>4.8300000000000003E-2</v>
+      </c>
+      <c r="N12">
+        <v>0.83189999999999997</v>
+      </c>
+      <c r="O12">
+        <v>0.82150000000000001</v>
+      </c>
+      <c r="P12">
+        <v>0.67679999999999996</v>
+      </c>
+      <c r="Q12">
+        <v>4.99E-2</v>
+      </c>
+      <c r="R12">
+        <v>0.68989999999999996</v>
+      </c>
+      <c r="S12">
+        <v>0.69259999999999999</v>
+      </c>
+      <c r="T12">
+        <v>0.4703</v>
+      </c>
+      <c r="U12">
+        <v>0.27589999999999998</v>
+      </c>
+      <c r="V12">
+        <v>0.2427</v>
+      </c>
+      <c r="W12">
+        <v>0.1767</v>
+      </c>
+      <c r="X12">
+        <v>0.55930000000000002</v>
+      </c>
+      <c r="Y12">
+        <v>0.55730000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:25">

</xml_diff>

<commit_message>
UPDATE result.xlsx and fix gae bugs
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qianzhiqiang/PycharmProjects/NetBenchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9719B5E1-1F67-F343-B4A6-8DDF954A5E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7083655D-2275-1740-9092-21C6F5E60D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="28240" windowHeight="16400" xr2:uid="{A9C37B03-D3ED-DD4C-96A1-B014332CD34F}"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="28240" windowHeight="16400" activeTab="1" xr2:uid="{A9C37B03-D3ED-DD4C-96A1-B014332CD34F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -244,6 +244,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -252,12 +258,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,7 +575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0428EAC-9C8D-1A4A-9ED3-B464BF9D83B8}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0">
+    <sheetView zoomScale="124" workbookViewId="0">
       <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
@@ -586,46 +586,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="7" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8" t="s">
+      <c r="K1" s="10"/>
+      <c r="L1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="8"/>
-      <c r="N1" s="6" t="s">
+      <c r="M1" s="10"/>
+      <c r="N1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="8" t="s">
+      <c r="O1" s="8"/>
+      <c r="P1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="6" t="s">
+      <c r="Q1" s="10"/>
+      <c r="R1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6" t="s">
+      <c r="S1" s="8"/>
+      <c r="T1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="6"/>
+      <c r="U1" s="8"/>
     </row>
     <row r="2" spans="1:21">
       <c r="B2" t="s">
@@ -1518,53 +1518,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B71108-CCFD-BD42-997A-0DECA2451E6F}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView zoomScale="138" zoomScaleNormal="138" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6" t="s">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6" t="s">
+      <c r="M1" s="8"/>
+      <c r="N1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6" t="s">
+      <c r="O1" s="8"/>
+      <c r="P1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6" t="s">
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6" t="s">
+      <c r="S1" s="8"/>
+      <c r="T1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="6"/>
+      <c r="U1" s="8"/>
     </row>
     <row r="2" spans="1:21">
       <c r="B2" t="s">
@@ -1780,8 +1780,8 @@
       <c r="G5">
         <v>0.85599999999999998</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
       <c r="J5">
         <v>0.85570000000000002</v>
       </c>
@@ -2224,16 +2224,22 @@
       <c r="C13">
         <v>0.74380000000000002</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
       <c r="F13">
         <v>0.75449999999999995</v>
       </c>
       <c r="G13">
         <v>0.74939999999999996</v>
       </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13">
+        <v>0.7661</v>
+      </c>
+      <c r="K13">
+        <v>0.78159999999999996</v>
+      </c>
       <c r="L13">
         <v>0.85980000000000001</v>
       </c>
@@ -2411,46 +2417,46 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6" t="s">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6" t="s">
+      <c r="M1" s="8"/>
+      <c r="N1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6" t="s">
+      <c r="O1" s="8"/>
+      <c r="P1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6" t="s">
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6" t="s">
+      <c r="S1" s="8"/>
+      <c r="T1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="6"/>
+      <c r="U1" s="8"/>
     </row>
     <row r="2" spans="1:21">
       <c r="B2" t="s">

</xml_diff>